<commit_message>
Validacion de carga de datos
</commit_message>
<xml_diff>
--- a/public/storage/archivo_datos/1511727996.xlsx
+++ b/public/storage/archivo_datos/1511727996.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Comisca\Dropbox\TG 23 2017\primera etapa\archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\sigve\public\storage\archivo_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>País:</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Centro para el tramiento de la tuberculosis</t>
-  </si>
-  <si>
-    <t>Belize</t>
   </si>
   <si>
     <t>Personas estimadas con VIH (SPECTRUM)</t>
@@ -295,6 +292,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -303,9 +303,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -593,7 +590,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,15 +609,15 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7">
         <v>2013</v>
@@ -628,7 +625,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -639,23 +636,23 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:10" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -663,13 +660,13 @@
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="17">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13">
         <v>43465</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -678,27 +675,27 @@
     <row r="7" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -739,11 +736,11 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -763,11 +760,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>